<commit_message>
Finish Delete All Buttons
</commit_message>
<xml_diff>
--- a/public/exportdata.xlsx
+++ b/public/exportdata.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -407,140 +407,111 @@
         <v>_id</v>
       </c>
       <c r="B1" t="str">
-        <v>precinct</v>
+        <v>fullname</v>
       </c>
       <c r="C1" t="str">
-        <v>daterecorded</v>
+        <v>username</v>
       </c>
       <c r="D1" t="str">
-        <v>lastname</v>
+        <v>email</v>
       </c>
       <c r="E1" t="str">
-        <v>firstname</v>
+        <v>accountrole</v>
       </c>
       <c r="F1" t="str">
-        <v>middleinitial</v>
+        <v>__v</v>
       </c>
       <c r="G1" t="str">
+        <v>address</v>
+      </c>
+      <c r="H1" t="str">
         <v>birthday</v>
       </c>
-      <c r="H1" t="str">
-        <v>birthplace</v>
-      </c>
       <c r="I1" t="str">
-        <v>age</v>
+        <v>phone</v>
       </c>
       <c r="J1" t="str">
-        <v>civilstatus</v>
-      </c>
-      <c r="K1" t="str">
-        <v>email</v>
-      </c>
-      <c r="L1" t="str">
-        <v>phone</v>
-      </c>
-      <c r="M1" t="str">
-        <v>schoolattainment</v>
-      </c>
-      <c r="N1" t="str">
-        <v>profession</v>
-      </c>
-      <c r="O1" t="str">
-        <v>blklot</v>
-      </c>
-      <c r="P1" t="str">
-        <v>street</v>
-      </c>
-      <c r="Q1" t="str">
-        <v>brgy</v>
-      </c>
-      <c r="R1" t="str">
-        <v>province</v>
-      </c>
-      <c r="S1" t="str">
-        <v>citizen</v>
-      </c>
-      <c r="T1" t="str">
-        <v>zipcode</v>
-      </c>
-      <c r="U1" t="str">
-        <v>__v</v>
-      </c>
-      <c r="V1" t="str">
-        <v>gender</v>
+        <v>password</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>625446a64e1eb631a55773a2</v>
+        <v>62557f02b9324784a2aa21f8</v>
       </c>
       <c r="B2" t="str">
-        <v xml:space="preserve"> </v>
+        <v xml:space="preserve">Park Roseann             </v>
       </c>
       <c r="C2" t="str">
-        <v xml:space="preserve">11 April 2022 </v>
+        <v>roseann</v>
       </c>
       <c r="D2" t="str">
-        <v xml:space="preserve">Nicanor </v>
+        <v>roseann@g.c</v>
       </c>
       <c r="E2" t="str">
-        <v xml:space="preserve">Juliet </v>
-      </c>
-      <c r="F2" t="str">
-        <v xml:space="preserve">M </v>
+        <v>admin</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
       </c>
       <c r="G2" t="str">
-        <v xml:space="preserve">20/12/1996 </v>
+        <v>South Korea</v>
       </c>
       <c r="H2" t="str">
-        <v xml:space="preserve">Angono, Rizal </v>
+        <v>02/16/1997</v>
       </c>
       <c r="I2" t="str">
-        <v xml:space="preserve">23 </v>
+        <v>59454</v>
       </c>
       <c r="J2" t="str">
-        <v>Single</v>
-      </c>
-      <c r="K2" t="str">
-        <v>julietnicanor1996@gmail.com</v>
-      </c>
-      <c r="L2" t="str">
-        <v xml:space="preserve">+639395029337 </v>
-      </c>
-      <c r="M2" t="str">
-        <v>Elementary</v>
-      </c>
-      <c r="N2" t="str">
-        <v xml:space="preserve">Student </v>
-      </c>
-      <c r="O2" t="str">
-        <v xml:space="preserve">Blk 8 Lot 1 </v>
-      </c>
-      <c r="P2" t="str">
-        <v xml:space="preserve">Rosario Village, Botong Francisco Ave </v>
-      </c>
-      <c r="Q2" t="str">
-        <v xml:space="preserve">Barangay San Isidro </v>
-      </c>
-      <c r="R2" t="str">
-        <v xml:space="preserve">Angono </v>
-      </c>
-      <c r="S2" t="str">
-        <v xml:space="preserve">Filipino </v>
-      </c>
-      <c r="T2" t="str">
-        <v xml:space="preserve">1930 </v>
-      </c>
-      <c r="U2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>6255810366248bbde36e8563</v>
+      </c>
+      <c r="B3" t="str">
+        <v>kun</v>
+      </c>
+      <c r="C3" t="str">
+        <v>kunx</v>
+      </c>
+      <c r="D3" t="str">
+        <v>kunx@g.c</v>
+      </c>
+      <c r="E3" t="str">
+        <v>employee</v>
+      </c>
+      <c r="F3">
         <v>0</v>
       </c>
-      <c r="V2" t="str">
-        <v>Female</v>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>625582820fec137040de7e78</v>
+      </c>
+      <c r="B4" t="str">
+        <v xml:space="preserve">   adminx   </v>
+      </c>
+      <c r="C4" t="str">
+        <v>adminx</v>
+      </c>
+      <c r="D4" t="str">
+        <v>adminx@g.c</v>
+      </c>
+      <c r="E4" t="str">
+        <v>admin</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="str">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:V2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>